<commit_message>
LFO-Analog: change caps for different frequency range
</commit_message>
<xml_diff>
--- a/modules/LFO-Analog/rates.xlsx
+++ b/modules/LFO-Analog/rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\LFO-Analog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E5EDFE-0A7B-4B35-B3CA-3E207CB3A46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AB6250-478D-4025-81C4-FF01BACC4EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4230" yWindow="1545" windowWidth="19095" windowHeight="10770" xr2:uid="{D6506DEB-166E-454B-B240-A9B168113276}"/>
   </bookViews>
@@ -101,13 +101,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,13 +443,10 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="8" width="9.140625" style="2"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -512,20 +507,20 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.37040000000000001</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>169.5</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>2.6997840172786178</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f t="shared" si="1"/>
         <v>5.8997050147492625E-3</v>
       </c>
@@ -533,7 +528,7 @@
         <f>B4/B3</f>
         <v>3.0303030303030303</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <f>C3/C4</f>
         <v>2.9859611231101515</v>
       </c>
@@ -560,7 +555,7 @@
         <f>B5/B4</f>
         <v>68</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <f>C4/C5</f>
         <v>69.886792452830193</v>
       </c>
@@ -569,33 +564,30 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>470</v>
       </c>
-      <c r="C6" s="4">
-        <f>C5*B5/B6</f>
-        <v>7.6680851063829786E-3</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="C6" s="3">
+        <v>8.0389999999999993E-3</v>
+      </c>
+      <c r="D6" s="2">
         <f>D5*B5/B6</f>
         <v>3.7674893617021277</v>
       </c>
-      <c r="E6" s="3">
-        <f t="shared" si="0"/>
-        <v>130.41065482796893</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>124.39358129120538</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="1"/>
         <v>0.26542875214601969</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>125</v>
+      <c r="C7" s="1"/>
+      <c r="E7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="F7" t="e">
         <f t="shared" si="1"/>
@@ -603,6 +595,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
       <c r="E8" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>

</xml_diff>

<commit_message>
update README for LFO-Analog and LFO-DigiVC
</commit_message>
<xml_diff>
--- a/modules/LFO-Analog/rates.xlsx
+++ b/modules/LFO-Analog/rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\LFO-Analog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AB6250-478D-4025-81C4-FF01BACC4EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AB578A-798A-4A99-8223-C4B8DCCA7AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="1545" windowWidth="19095" windowHeight="10770" xr2:uid="{D6506DEB-166E-454B-B240-A9B168113276}"/>
+    <workbookView xWindow="765" yWindow="1710" windowWidth="19095" windowHeight="10770" xr2:uid="{D6506DEB-166E-454B-B240-A9B168113276}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Freq-lo</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Cap nF</t>
-  </si>
-  <si>
-    <t>(calculated)</t>
   </si>
 </sst>
 </file>
@@ -442,9 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C756BA5-79D7-4FC1-94A6-557AF60B1829}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -561,9 +556,6 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
       <c r="B6" s="2">
         <v>470</v>
       </c>

</xml_diff>